<commit_message>
data: Add the data files.
</commit_message>
<xml_diff>
--- a/data/general_statics-2023.xlsx
+++ b/data/general_statics-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\zivmax\CUMCM_2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8BCA9F-4156-410F-A016-BBF41829E0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12593A44-2DDF-4D17-BB59-5B03B3870C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9744" yWindow="4428" windowWidth="19176" windowHeight="9996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25510" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023年统计的相关数据" sheetId="5" r:id="rId1"/>
@@ -1764,7 +1764,9 @@
   </sheetPr>
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>